<commit_message>
Changed Excel file to hide name
</commit_message>
<xml_diff>
--- a/ReplicationStudy.xlsx
+++ b/ReplicationStudy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigo-e/Dropbox/NAIST/IWESEP2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75694F34-F912-9547-B6C5-D010EEF46123}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC92AAF-40FC-174D-89B9-D1D4477828C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="19780" activeTab="2" xr2:uid="{B503D126-77A2-C043-9DDA-323B5B7BC9A6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{B503D126-77A2-C043-9DDA-323B5B7BC9A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2498,7 +2498,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="3200" b="1"/>
-              <a:t>Current Work Results (Sōji Tantei)</a:t>
+              <a:t>Current Work Results ()</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -9199,7 +9199,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F8B2E111-B1B0-BF4A-8747-79F6FC7299C4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11661,7 +11661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3668F67B-FFC3-2347-A3A2-5171A29CCB06}">
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>